<commit_message>
Rearranged columns in example files, formatting changes
</commit_message>
<xml_diff>
--- a/tetramer_validator/static/sample.xlsx
+++ b/tetramer_validator/static/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amody/tetramer-validator/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amody/tetramer-validator/tetramer_validator/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127FE5B6-B036-9A4A-8C91-55A4145B3AD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432A82C8-E3EE-7A4E-8BC1-AB033B4A4CED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="3920" windowWidth="26840" windowHeight="15940" xr2:uid="{75EA4563-2D60-EC4A-8450-2866E5CE21DF}"/>
+    <workbookView xWindow="8800" yWindow="5760" windowWidth="26840" windowHeight="15940" xr2:uid="{75EA4563-2D60-EC4A-8450-2866E5CE21DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,21 +73,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -95,28 +89,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -435,7 +413,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,19 +447,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>